<commit_message>
update correlation and regression
</commit_message>
<xml_diff>
--- a/tabla_descriptivos_1.xlsx
+++ b/tabla_descriptivos_1.xlsx
@@ -401,10 +401,10 @@
         <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>55.6</v>
+        <v>9.26666666666667</v>
       </c>
       <c r="E2" t="n">
-        <v>6.59622650320868</v>
+        <v>1.09937108386811</v>
       </c>
     </row>
     <row r="3">
@@ -418,10 +418,10 @@
         <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>53.25</v>
+        <v>8.875</v>
       </c>
       <c r="E3" t="n">
-        <v>7.08444732773093</v>
+        <v>1.18074122128849</v>
       </c>
     </row>
     <row r="4">
@@ -435,10 +435,10 @@
         <v>100</v>
       </c>
       <c r="D4" t="n">
-        <v>51.8</v>
+        <v>8.69</v>
       </c>
       <c r="E4" t="n">
-        <v>10.3113157416128</v>
+        <v>1.69388879778433</v>
       </c>
     </row>
     <row r="5">
@@ -452,10 +452,10 @@
         <v>50</v>
       </c>
       <c r="D5" t="n">
-        <v>45</v>
+        <v>7.5</v>
       </c>
       <c r="E5" t="n">
-        <v>13.6650903355064</v>
+        <v>2.27751505591774</v>
       </c>
     </row>
     <row r="6">
@@ -469,10 +469,10 @@
         <v>100</v>
       </c>
       <c r="D6" t="n">
-        <v>44.35</v>
+        <v>7.39166666666667</v>
       </c>
       <c r="E6" t="n">
-        <v>13.2126164071781</v>
+        <v>2.20210273452969</v>
       </c>
     </row>
     <row r="7">
@@ -486,10 +486,10 @@
         <v>100</v>
       </c>
       <c r="D7" t="n">
-        <v>41.9</v>
+        <v>7.02833333333333</v>
       </c>
       <c r="E7" t="n">
-        <v>15.903433337465</v>
+        <v>2.65052511579311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>